<commit_message>
Bug fixes on deformable protopnet
</commit_message>
<xml_diff>
--- a/paper/paper_acc_results.xlsx
+++ b/paper/paper_acc_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiagofilipesousagoncalves/Desktop/GitHub/proto-counterfactuals/paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA6048A-7801-EC40-B1C6-304D636708FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B15D22-DF75-E64C-ACE9-4B890276C293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CUB2002011" sheetId="1" r:id="rId1"/>
@@ -518,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1361,7 +1361,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="N12" sqref="N12:N14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated: compute_counterfactual_label_coherence.sh, cub2002011_counterfactual_retrieval.sh, paper/paper_acc_results.xlsx, papila_counterfactual_retrieval.sh, ph2_counterfactual_retrieval.sh
</commit_message>
<xml_diff>
--- a/paper/paper_acc_results.xlsx
+++ b/paper/paper_acc_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiagofilipesousagoncalves/Desktop/GitHub/proto-counterfactuals/paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26B7B93-169E-124B-88CD-9FD8CB7B93EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FBB8CFE-9734-4042-ACD3-3FB7FA2ED829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17860" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CUB2002011" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="47">
   <si>
     <t>ProtoPNet</t>
   </si>
@@ -103,36 +103,24 @@
     <t>2023-01-04_12-12-15</t>
   </si>
   <si>
-    <t>2023-01-16_00-08-15</t>
-  </si>
-  <si>
     <t>2022-12-23_18-42-05</t>
   </si>
   <si>
     <t>2023-01-04_16-02-21</t>
   </si>
   <si>
-    <t>2023-01-16_07-33-46</t>
-  </si>
-  <si>
     <t>2022-12-23_18-10-15</t>
   </si>
   <si>
     <t>2023-01-04_18-47-51</t>
   </si>
   <si>
-    <t>2023-01-16_13-44-00</t>
-  </si>
-  <si>
     <t>2022-12-06_15-51-53</t>
   </si>
   <si>
     <t>2023-01-02_08-43-56</t>
   </si>
   <si>
-    <t>2023-01-16_20-22-43</t>
-  </si>
-  <si>
     <t>2022-12-06_19-46-07</t>
   </si>
   <si>
@@ -142,9 +130,6 @@
     <t>2023-01-02_10-08-37</t>
   </si>
   <si>
-    <t>2023-01-16_22-56-35</t>
-  </si>
-  <si>
     <t>2022-12-07_00-40-00</t>
   </si>
   <si>
@@ -154,19 +139,31 @@
     <t>2023-01-04_10-43-58</t>
   </si>
   <si>
-    <t>2023-01-17_01-29-53</t>
-  </si>
-  <si>
     <t>2022-12-07_02-48-40</t>
   </si>
   <si>
-    <t>2023-01-17_03-44-38</t>
-  </si>
-  <si>
-    <t>2023-01-21_03-37-39</t>
-  </si>
-  <si>
-    <t>2023-01-24_01-40-54</t>
+    <t>2023-03-28_14-00-03</t>
+  </si>
+  <si>
+    <t>2023-03-29_23-07-14</t>
+  </si>
+  <si>
+    <t>2023-03-28_13-59-11</t>
+  </si>
+  <si>
+    <t>2023-03-28_13-59-15</t>
+  </si>
+  <si>
+    <t>2023-03-28_13-59-24</t>
+  </si>
+  <si>
+    <t>2023-03-28_13-59-31</t>
+  </si>
+  <si>
+    <t>2023-03-28_18-16-50</t>
+  </si>
+  <si>
+    <t>2023-03-29_15-36-45</t>
   </si>
 </sst>
 </file>
@@ -232,10 +229,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -518,7 +515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -542,27 +539,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="G1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="M1" s="7" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="G1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="M1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -612,10 +609,10 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
@@ -627,10 +624,10 @@
       <c r="E3" s="4">
         <v>0.76803589920607496</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="7" t="s">
         <v>9</v>
       </c>
       <c r="I3" t="s">
@@ -642,10 +639,10 @@
       <c r="K3" s="5">
         <v>0.78598550224370001</v>
       </c>
-      <c r="M3" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="N3" s="6" t="s">
+      <c r="M3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="N3" s="7" t="s">
         <v>9</v>
       </c>
       <c r="O3" t="s">
@@ -655,12 +652,12 @@
         <v>1</v>
       </c>
       <c r="Q3" s="5">
-        <v>0.74767000345184598</v>
+        <v>0.74093890231273696</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
       <c r="C4" t="s">
         <v>13</v>
       </c>
@@ -670,8 +667,8 @@
       <c r="E4" s="4">
         <v>0.76044183638246399</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
       <c r="I4" t="s">
         <v>13</v>
       </c>
@@ -681,8 +678,8 @@
       <c r="K4" s="5">
         <v>0.77459440800828405</v>
       </c>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
       <c r="O4" t="s">
         <v>13</v>
       </c>
@@ -694,8 +691,8 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
       <c r="C5" t="s">
         <v>14</v>
       </c>
@@ -705,8 +702,8 @@
       <c r="E5" s="4">
         <v>0.76372109078356898</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
       <c r="I5" t="s">
         <v>14</v>
       </c>
@@ -716,8 +713,8 @@
       <c r="K5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
       <c r="O5" t="s">
         <v>14</v>
       </c>
@@ -725,14 +722,14 @@
         <v>1</v>
       </c>
       <c r="Q5" s="5">
-        <v>0.75077666551605104</v>
+        <v>0.74577148774594404</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C6" t="s">
@@ -744,10 +741,10 @@
       <c r="E6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="6" t="s">
+      <c r="G6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I6" t="s">
@@ -759,10 +756,10 @@
       <c r="K6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="N6" s="6" t="s">
+      <c r="M6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N6" s="7" t="s">
         <v>15</v>
       </c>
       <c r="O6" t="s">
@@ -776,8 +773,8 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
       <c r="C7" t="s">
         <v>13</v>
       </c>
@@ -787,8 +784,8 @@
       <c r="E7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
       <c r="I7" t="s">
         <v>13</v>
       </c>
@@ -798,8 +795,8 @@
       <c r="K7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
       <c r="O7" t="s">
         <v>13</v>
       </c>
@@ -811,8 +808,8 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
       <c r="C8" t="s">
         <v>14</v>
       </c>
@@ -822,8 +819,8 @@
       <c r="E8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
       <c r="I8" t="s">
         <v>14</v>
       </c>
@@ -833,8 +830,8 @@
       <c r="K8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
       <c r="O8" t="s">
         <v>14</v>
       </c>
@@ -846,10 +843,10 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C9" t="s">
@@ -861,10 +858,10 @@
       <c r="E9" s="4">
         <v>0.783741801863997</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="7" t="s">
         <v>17</v>
       </c>
       <c r="I9" t="s">
@@ -876,25 +873,25 @@
       <c r="K9" s="5">
         <v>0.74473593372454205</v>
       </c>
-      <c r="M9" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="N9" s="6" t="s">
+      <c r="M9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="N9" s="7" t="s">
         <v>17</v>
       </c>
       <c r="O9" t="s">
         <v>10</v>
       </c>
       <c r="P9" s="5">
-        <v>0.99432766099432701</v>
+        <v>1</v>
       </c>
       <c r="Q9" s="5">
-        <v>0.73403520883672702</v>
+        <v>0.71677597514670299</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
       <c r="C10" t="s">
         <v>13</v>
       </c>
@@ -904,8 +901,8 @@
       <c r="E10" s="4">
         <v>0.77217811529168101</v>
       </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
       <c r="I10" t="s">
         <v>13</v>
       </c>
@@ -915,8 +912,8 @@
       <c r="K10" s="5">
         <v>0.74542630307214297</v>
       </c>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
       <c r="O10" t="s">
         <v>13</v>
       </c>
@@ -928,8 +925,8 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
       <c r="C11" t="s">
         <v>14</v>
       </c>
@@ -939,8 +936,8 @@
       <c r="E11" s="4">
         <v>0.77735588539868805</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
       <c r="I11" t="s">
         <v>14</v>
       </c>
@@ -950,8 +947,8 @@
       <c r="K11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
       <c r="O11" t="s">
         <v>14</v>
       </c>
@@ -959,14 +956,14 @@
         <v>1</v>
       </c>
       <c r="Q11" s="5">
-        <v>0.73886779426993399</v>
+        <v>0.71850189851570501</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="6" t="s">
+      <c r="A12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C12" t="s">
@@ -978,10 +975,10 @@
       <c r="E12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="6" t="s">
+      <c r="G12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="7" t="s">
         <v>19</v>
       </c>
       <c r="I12" t="s">
@@ -993,10 +990,10 @@
       <c r="K12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="N12" s="6" t="s">
+      <c r="M12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N12" s="7" t="s">
         <v>19</v>
       </c>
       <c r="O12" t="s">
@@ -1010,8 +1007,8 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
       <c r="C13" t="s">
         <v>13</v>
       </c>
@@ -1021,8 +1018,8 @@
       <c r="E13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
       <c r="I13" t="s">
         <v>13</v>
       </c>
@@ -1032,8 +1029,8 @@
       <c r="K13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
       <c r="O13" t="s">
         <v>13</v>
       </c>
@@ -1045,8 +1042,8 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
       <c r="C14" t="s">
         <v>14</v>
       </c>
@@ -1056,8 +1053,8 @@
       <c r="E14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
       <c r="I14" t="s">
         <v>14</v>
       </c>
@@ -1067,8 +1064,8 @@
       <c r="K14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
       <c r="O14" t="s">
         <v>14</v>
       </c>
@@ -1080,10 +1077,10 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C15" t="s">
@@ -1095,10 +1092,10 @@
       <c r="E15" s="4">
         <v>0.75768035899205999</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="7" t="s">
         <v>21</v>
       </c>
       <c r="I15" t="s">
@@ -1110,25 +1107,25 @@
       <c r="K15" s="5">
         <v>0.73990334829133497</v>
       </c>
-      <c r="M15" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="N15" s="6" t="s">
+      <c r="M15" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="N15" s="7" t="s">
         <v>21</v>
       </c>
       <c r="O15" t="s">
         <v>10</v>
       </c>
       <c r="P15" s="5">
-        <v>0.99265932599265905</v>
+        <v>1</v>
       </c>
       <c r="Q15" s="5">
-        <v>0.61080428028995504</v>
+        <v>0.66534345875043099</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
       <c r="C16" t="s">
         <v>13</v>
       </c>
@@ -1138,8 +1135,8 @@
       <c r="E16" s="4">
         <v>0.73403520883672702</v>
       </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
       <c r="I16" t="s">
         <v>13</v>
       </c>
@@ -1149,8 +1146,8 @@
       <c r="K16" s="5">
         <v>0.71505005177770098</v>
       </c>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
       <c r="O16" t="s">
         <v>13</v>
       </c>
@@ -1162,8 +1159,8 @@
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
       <c r="C17" t="s">
         <v>14</v>
       </c>
@@ -1173,8 +1170,8 @@
       <c r="E17" s="4">
         <v>0.73835001725923299</v>
       </c>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
       <c r="I17" t="s">
         <v>14</v>
       </c>
@@ -1182,8 +1179,8 @@
         <v>12</v>
       </c>
       <c r="K17" s="5"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
       <c r="O17" t="s">
         <v>14</v>
       </c>
@@ -1191,14 +1188,14 @@
         <v>1</v>
       </c>
       <c r="Q17" s="5">
-        <v>0.62409389023127304</v>
+        <v>0.62340352088367201</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="6" t="s">
+      <c r="A18" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>23</v>
       </c>
       <c r="C18" t="s">
@@ -1210,10 +1207,10 @@
       <c r="E18" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G18" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H18" s="6" t="s">
+      <c r="G18" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="7" t="s">
         <v>23</v>
       </c>
       <c r="I18" t="s">
@@ -1225,10 +1222,10 @@
       <c r="K18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M18" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="N18" s="6" t="s">
+      <c r="M18" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N18" s="7" t="s">
         <v>23</v>
       </c>
       <c r="O18" t="s">
@@ -1242,8 +1239,8 @@
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
       <c r="C19" t="s">
         <v>13</v>
       </c>
@@ -1253,8 +1250,8 @@
       <c r="E19" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
       <c r="I19" t="s">
         <v>13</v>
       </c>
@@ -1264,8 +1261,8 @@
       <c r="K19" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
       <c r="O19" t="s">
         <v>13</v>
       </c>
@@ -1277,8 +1274,8 @@
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
       <c r="C20" t="s">
         <v>14</v>
       </c>
@@ -1288,8 +1285,8 @@
       <c r="E20" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
       <c r="I20" t="s">
         <v>14</v>
       </c>
@@ -1299,8 +1296,8 @@
       <c r="K20" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
       <c r="O20" t="s">
         <v>14</v>
       </c>
@@ -1313,15 +1310,26 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="M1:Q1"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="G3:G5"/>
-    <mergeCell ref="G6:G8"/>
-    <mergeCell ref="M3:M5"/>
-    <mergeCell ref="M6:M8"/>
+    <mergeCell ref="M9:M11"/>
+    <mergeCell ref="M12:M14"/>
+    <mergeCell ref="M15:M17"/>
+    <mergeCell ref="M18:M20"/>
+    <mergeCell ref="N3:N5"/>
+    <mergeCell ref="N6:N8"/>
+    <mergeCell ref="N9:N11"/>
+    <mergeCell ref="N12:N14"/>
+    <mergeCell ref="N15:N17"/>
+    <mergeCell ref="N18:N20"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="G12:G14"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="H3:H5"/>
+    <mergeCell ref="H6:H8"/>
+    <mergeCell ref="H9:H11"/>
+    <mergeCell ref="H12:H14"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="H18:H20"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A15:A17"/>
@@ -1332,26 +1340,15 @@
     <mergeCell ref="B12:B14"/>
     <mergeCell ref="B15:B17"/>
     <mergeCell ref="B18:B20"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="G12:G14"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="H3:H5"/>
-    <mergeCell ref="H6:H8"/>
-    <mergeCell ref="H9:H11"/>
-    <mergeCell ref="H12:H14"/>
-    <mergeCell ref="H15:H17"/>
-    <mergeCell ref="H18:H20"/>
-    <mergeCell ref="M9:M11"/>
-    <mergeCell ref="M12:M14"/>
-    <mergeCell ref="M15:M17"/>
-    <mergeCell ref="M18:M20"/>
-    <mergeCell ref="N3:N5"/>
-    <mergeCell ref="N6:N8"/>
-    <mergeCell ref="N9:N11"/>
-    <mergeCell ref="N12:N14"/>
-    <mergeCell ref="N15:N17"/>
-    <mergeCell ref="N18:N20"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="M1:Q1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="G6:G8"/>
+    <mergeCell ref="M3:M5"/>
+    <mergeCell ref="M6:M8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1362,7 +1359,7 @@
   <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="E1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1385,27 +1382,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="G1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="M1" s="7" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="G1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="M1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1455,7 +1452,7 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -1470,7 +1467,7 @@
       <c r="E3" s="4">
         <v>0.75</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="7" t="s">
         <v>25</v>
       </c>
       <c r="H3" s="8" t="s">
@@ -1485,8 +1482,8 @@
       <c r="K3" s="5">
         <v>0.81081081081080997</v>
       </c>
-      <c r="M3" s="6" t="s">
-        <v>26</v>
+      <c r="M3" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="N3" s="8" t="s">
         <v>9</v>
@@ -1495,14 +1492,14 @@
         <v>10</v>
       </c>
       <c r="P3" s="5">
-        <v>1</v>
+        <v>0.98823529411764699</v>
       </c>
       <c r="Q3" s="5">
-        <v>0.80405405405405395</v>
+        <v>0.77702702702702697</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="8"/>
       <c r="C4" t="s">
         <v>13</v>
@@ -1513,7 +1510,7 @@
       <c r="E4" s="4">
         <v>0.76351351351351304</v>
       </c>
-      <c r="G4" s="6"/>
+      <c r="G4" s="7"/>
       <c r="H4" s="8"/>
       <c r="I4" t="s">
         <v>13</v>
@@ -1524,7 +1521,7 @@
       <c r="K4" s="5">
         <v>0.80405405405405395</v>
       </c>
-      <c r="M4" s="6"/>
+      <c r="M4" s="7"/>
       <c r="N4" s="8"/>
       <c r="O4" t="s">
         <v>13</v>
@@ -1537,7 +1534,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="8"/>
       <c r="C5" t="s">
         <v>14</v>
@@ -1548,7 +1545,7 @@
       <c r="E5" s="4">
         <v>0.75675675675675602</v>
       </c>
-      <c r="G5" s="6"/>
+      <c r="G5" s="7"/>
       <c r="H5" s="8"/>
       <c r="I5" t="s">
         <v>14</v>
@@ -1559,7 +1556,7 @@
       <c r="K5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="6"/>
+      <c r="M5" s="7"/>
       <c r="N5" s="8"/>
       <c r="O5" t="s">
         <v>14</v>
@@ -1568,14 +1565,14 @@
         <v>1</v>
       </c>
       <c r="Q5" s="5">
-        <v>0.81081081081080997</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C6" t="s">
@@ -1587,10 +1584,10 @@
       <c r="E6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="6" t="s">
+      <c r="G6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I6" t="s">
@@ -1602,10 +1599,10 @@
       <c r="K6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="N6" s="6" t="s">
+      <c r="M6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N6" s="7" t="s">
         <v>15</v>
       </c>
       <c r="O6" t="s">
@@ -1619,8 +1616,8 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
       <c r="C7" t="s">
         <v>13</v>
       </c>
@@ -1630,8 +1627,8 @@
       <c r="E7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
       <c r="I7" t="s">
         <v>13</v>
       </c>
@@ -1641,8 +1638,8 @@
       <c r="K7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
       <c r="O7" t="s">
         <v>13</v>
       </c>
@@ -1654,8 +1651,8 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
       <c r="C8" t="s">
         <v>14</v>
       </c>
@@ -1665,8 +1662,8 @@
       <c r="E8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
       <c r="I8" t="s">
         <v>14</v>
       </c>
@@ -1676,8 +1673,8 @@
       <c r="K8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
       <c r="O8" t="s">
         <v>14</v>
       </c>
@@ -1689,10 +1686,10 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="6" t="s">
+      <c r="A9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C9" t="s">
@@ -1704,10 +1701,10 @@
       <c r="E9" s="4">
         <v>0.75</v>
       </c>
-      <c r="G9" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" s="6" t="s">
+      <c r="G9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="7" t="s">
         <v>17</v>
       </c>
       <c r="I9" t="s">
@@ -1719,10 +1716,10 @@
       <c r="K9" s="5">
         <v>0.80405405405405395</v>
       </c>
-      <c r="M9" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="N9" s="6" t="s">
+      <c r="M9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="N9" s="7" t="s">
         <v>17</v>
       </c>
       <c r="O9" t="s">
@@ -1732,12 +1729,12 @@
         <v>1</v>
       </c>
       <c r="Q9" s="5">
-        <v>0.79054054054054002</v>
+        <v>0.77027027027026995</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
       <c r="C10" t="s">
         <v>13</v>
       </c>
@@ -1747,8 +1744,8 @@
       <c r="E10" s="4">
         <v>0.72972972972972905</v>
       </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
       <c r="I10" t="s">
         <v>13</v>
       </c>
@@ -1758,8 +1755,8 @@
       <c r="K10" s="5">
         <v>0.75675675675675602</v>
       </c>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
       <c r="O10" t="s">
         <v>13</v>
       </c>
@@ -1771,8 +1768,8 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
       <c r="C11" t="s">
         <v>14</v>
       </c>
@@ -1782,8 +1779,8 @@
       <c r="E11" s="4">
         <v>0.72972972972972905</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
       <c r="I11" t="s">
         <v>14</v>
       </c>
@@ -1791,8 +1788,8 @@
         <v>12</v>
       </c>
       <c r="K11" s="5"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
       <c r="O11" t="s">
         <v>14</v>
       </c>
@@ -1800,14 +1797,14 @@
         <v>1</v>
       </c>
       <c r="Q11" s="5">
-        <v>0.80405405405405395</v>
+        <v>0.76351351351351304</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="6" t="s">
+      <c r="A12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C12" t="s">
@@ -1819,10 +1816,10 @@
       <c r="E12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="6" t="s">
+      <c r="G12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="7" t="s">
         <v>19</v>
       </c>
       <c r="I12" t="s">
@@ -1834,10 +1831,10 @@
       <c r="K12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="N12" s="6" t="s">
+      <c r="M12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N12" s="7" t="s">
         <v>19</v>
       </c>
       <c r="O12" t="s">
@@ -1851,8 +1848,8 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
       <c r="C13" t="s">
         <v>13</v>
       </c>
@@ -1862,8 +1859,8 @@
       <c r="E13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
       <c r="I13" t="s">
         <v>13</v>
       </c>
@@ -1873,8 +1870,8 @@
       <c r="K13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
       <c r="O13" t="s">
         <v>13</v>
       </c>
@@ -1886,8 +1883,8 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
       <c r="C14" t="s">
         <v>14</v>
       </c>
@@ -1897,8 +1894,8 @@
       <c r="E14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
       <c r="I14" t="s">
         <v>14</v>
       </c>
@@ -1908,8 +1905,8 @@
       <c r="K14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
       <c r="O14" t="s">
         <v>14</v>
       </c>
@@ -1921,10 +1918,10 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="6" t="s">
+      <c r="A15" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C15" t="s">
@@ -1936,10 +1933,10 @@
       <c r="E15" s="4">
         <v>0.75</v>
       </c>
-      <c r="G15" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H15" s="6" t="s">
+      <c r="G15" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15" s="7" t="s">
         <v>21</v>
       </c>
       <c r="I15" t="s">
@@ -1951,10 +1948,10 @@
       <c r="K15" s="5">
         <v>0.76351351351351304</v>
       </c>
-      <c r="M15" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="N15" s="6" t="s">
+      <c r="M15" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="N15" s="7" t="s">
         <v>21</v>
       </c>
       <c r="O15" t="s">
@@ -1964,12 +1961,12 @@
         <v>0.997058823529411</v>
       </c>
       <c r="Q15" s="5">
-        <v>0.77027027027026995</v>
+        <v>0.77702702702702697</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
       <c r="C16" t="s">
         <v>13</v>
       </c>
@@ -1979,8 +1976,8 @@
       <c r="E16" s="4">
         <v>0.76351351351351304</v>
       </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
       <c r="I16" t="s">
         <v>13</v>
       </c>
@@ -1990,8 +1987,8 @@
       <c r="K16" s="5">
         <v>0.74324324324324298</v>
       </c>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
       <c r="O16" t="s">
         <v>13</v>
       </c>
@@ -2003,8 +2000,8 @@
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
       <c r="C17" t="s">
         <v>14</v>
       </c>
@@ -2014,8 +2011,8 @@
       <c r="E17" s="4">
         <v>0.75675675675675602</v>
       </c>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
       <c r="I17" t="s">
         <v>14</v>
       </c>
@@ -2025,8 +2022,8 @@
       <c r="K17" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
       <c r="O17" t="s">
         <v>14</v>
       </c>
@@ -2034,14 +2031,14 @@
         <v>1</v>
       </c>
       <c r="Q17" s="5">
-        <v>0.75</v>
+        <v>0.77027027027026995</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="6" t="s">
+      <c r="A18" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>23</v>
       </c>
       <c r="C18" t="s">
@@ -2053,10 +2050,10 @@
       <c r="E18" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G18" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H18" s="6" t="s">
+      <c r="G18" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="7" t="s">
         <v>23</v>
       </c>
       <c r="I18" t="s">
@@ -2068,10 +2065,10 @@
       <c r="K18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M18" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="N18" s="6" t="s">
+      <c r="M18" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N18" s="7" t="s">
         <v>23</v>
       </c>
       <c r="O18" t="s">
@@ -2085,8 +2082,8 @@
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
       <c r="C19" t="s">
         <v>13</v>
       </c>
@@ -2096,8 +2093,8 @@
       <c r="E19" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
       <c r="I19" t="s">
         <v>13</v>
       </c>
@@ -2107,8 +2104,8 @@
       <c r="K19" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
       <c r="O19" t="s">
         <v>13</v>
       </c>
@@ -2120,8 +2117,8 @@
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
       <c r="C20" t="s">
         <v>14</v>
       </c>
@@ -2131,8 +2128,8 @@
       <c r="E20" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
       <c r="I20" t="s">
         <v>14</v>
       </c>
@@ -2142,8 +2139,8 @@
       <c r="K20" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
       <c r="O20" t="s">
         <v>14</v>
       </c>
@@ -2156,15 +2153,26 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="M1:Q1"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="G3:G5"/>
-    <mergeCell ref="G6:G8"/>
-    <mergeCell ref="M3:M5"/>
-    <mergeCell ref="M6:M8"/>
+    <mergeCell ref="M9:M11"/>
+    <mergeCell ref="M12:M14"/>
+    <mergeCell ref="M15:M17"/>
+    <mergeCell ref="M18:M20"/>
+    <mergeCell ref="N3:N5"/>
+    <mergeCell ref="N6:N8"/>
+    <mergeCell ref="N9:N11"/>
+    <mergeCell ref="N12:N14"/>
+    <mergeCell ref="N15:N17"/>
+    <mergeCell ref="N18:N20"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="G12:G14"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="H3:H5"/>
+    <mergeCell ref="H6:H8"/>
+    <mergeCell ref="H9:H11"/>
+    <mergeCell ref="H12:H14"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="H18:H20"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A15:A17"/>
@@ -2175,26 +2183,15 @@
     <mergeCell ref="B12:B14"/>
     <mergeCell ref="B15:B17"/>
     <mergeCell ref="B18:B20"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="G12:G14"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="H3:H5"/>
-    <mergeCell ref="H6:H8"/>
-    <mergeCell ref="H9:H11"/>
-    <mergeCell ref="H12:H14"/>
-    <mergeCell ref="H15:H17"/>
-    <mergeCell ref="H18:H20"/>
-    <mergeCell ref="M9:M11"/>
-    <mergeCell ref="M12:M14"/>
-    <mergeCell ref="M15:M17"/>
-    <mergeCell ref="M18:M20"/>
-    <mergeCell ref="N3:N5"/>
-    <mergeCell ref="N6:N8"/>
-    <mergeCell ref="N9:N11"/>
-    <mergeCell ref="N12:N14"/>
-    <mergeCell ref="N15:N17"/>
-    <mergeCell ref="N18:N20"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="M1:Q1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="G6:G8"/>
+    <mergeCell ref="M3:M5"/>
+    <mergeCell ref="M6:M8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2228,27 +2225,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="G1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="M1" s="7" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="G1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="M1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -2298,8 +2295,8 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>33</v>
+      <c r="A3" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>9</v>
@@ -2313,8 +2310,8 @@
       <c r="E3" s="4">
         <v>0.73333333333333295</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>34</v>
+      <c r="G3" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>9</v>
@@ -2328,8 +2325,8 @@
       <c r="K3" s="5">
         <v>0.71666666666666601</v>
       </c>
-      <c r="M3" s="6" t="s">
-        <v>35</v>
+      <c r="M3" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="N3" s="8" t="s">
         <v>9</v>
@@ -2341,11 +2338,11 @@
         <v>1</v>
       </c>
       <c r="Q3" s="5">
-        <v>0.71666666666666601</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="8"/>
       <c r="C4" t="s">
         <v>13</v>
@@ -2356,7 +2353,7 @@
       <c r="E4" s="4">
         <v>0.71666666666666601</v>
       </c>
-      <c r="G4" s="6"/>
+      <c r="G4" s="7"/>
       <c r="H4" s="8"/>
       <c r="I4" t="s">
         <v>13</v>
@@ -2367,7 +2364,7 @@
       <c r="K4" s="5">
         <v>0.66666666666666596</v>
       </c>
-      <c r="M4" s="6"/>
+      <c r="M4" s="7"/>
       <c r="N4" s="8"/>
       <c r="O4" t="s">
         <v>13</v>
@@ -2380,7 +2377,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="8"/>
       <c r="C5" t="s">
         <v>14</v>
@@ -2391,7 +2388,7 @@
       <c r="E5" s="4">
         <v>0.73333333333333295</v>
       </c>
-      <c r="G5" s="6"/>
+      <c r="G5" s="7"/>
       <c r="H5" s="8"/>
       <c r="I5" t="s">
         <v>14</v>
@@ -2402,7 +2399,7 @@
       <c r="K5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="6"/>
+      <c r="M5" s="7"/>
       <c r="N5" s="8"/>
       <c r="O5" t="s">
         <v>14</v>
@@ -2411,14 +2408,14 @@
         <v>1</v>
       </c>
       <c r="Q5" s="5">
-        <v>0.7</v>
+        <v>0.66666666666666596</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C6" t="s">
@@ -2430,10 +2427,10 @@
       <c r="E6" s="4">
         <v>0.71666666666666601</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="6" t="s">
+      <c r="G6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I6" t="s">
@@ -2445,10 +2442,10 @@
       <c r="K6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="N6" s="6" t="s">
+      <c r="M6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N6" s="7" t="s">
         <v>15</v>
       </c>
       <c r="O6" t="s">
@@ -2462,8 +2459,8 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
       <c r="C7" t="s">
         <v>13</v>
       </c>
@@ -2473,8 +2470,8 @@
       <c r="E7" s="4">
         <v>0.7</v>
       </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
       <c r="I7" t="s">
         <v>13</v>
       </c>
@@ -2484,8 +2481,8 @@
       <c r="K7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
       <c r="O7" t="s">
         <v>13</v>
       </c>
@@ -2497,8 +2494,8 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
       <c r="C8" t="s">
         <v>14</v>
       </c>
@@ -2508,8 +2505,8 @@
       <c r="E8" s="4">
         <v>0.71666666666666601</v>
       </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
       <c r="I8" t="s">
         <v>14</v>
       </c>
@@ -2519,8 +2516,8 @@
       <c r="K8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
       <c r="O8" t="s">
         <v>14</v>
       </c>
@@ -2532,10 +2529,10 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="6" t="s">
+      <c r="A9" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C9" t="s">
@@ -2547,10 +2544,10 @@
       <c r="E9" s="4">
         <v>0.76666666666666605</v>
       </c>
-      <c r="G9" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="H9" s="6" t="s">
+      <c r="G9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="7" t="s">
         <v>17</v>
       </c>
       <c r="I9" t="s">
@@ -2562,10 +2559,10 @@
       <c r="K9" s="5">
         <v>0.68333333333333302</v>
       </c>
-      <c r="M9" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="N9" s="6" t="s">
+      <c r="M9" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="N9" s="7" t="s">
         <v>17</v>
       </c>
       <c r="O9" t="s">
@@ -2575,12 +2572,12 @@
         <v>1</v>
       </c>
       <c r="Q9" s="5">
-        <v>0.71666666666666601</v>
+        <v>0.66666666666666596</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
       <c r="C10" t="s">
         <v>13</v>
       </c>
@@ -2590,8 +2587,8 @@
       <c r="E10" s="4">
         <v>0.71666666666666601</v>
       </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
       <c r="I10" t="s">
         <v>13</v>
       </c>
@@ -2601,8 +2598,8 @@
       <c r="K10" s="5">
         <v>0.58333333333333304</v>
       </c>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
       <c r="O10" t="s">
         <v>13</v>
       </c>
@@ -2614,8 +2611,8 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
       <c r="C11" t="s">
         <v>14</v>
       </c>
@@ -2625,8 +2622,8 @@
       <c r="E11" s="4">
         <v>0.75</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
       <c r="I11" t="s">
         <v>14</v>
       </c>
@@ -2636,8 +2633,8 @@
       <c r="K11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
       <c r="O11" t="s">
         <v>14</v>
       </c>
@@ -2645,14 +2642,14 @@
         <v>1</v>
       </c>
       <c r="Q11" s="5">
-        <v>0.71666666666666601</v>
+        <v>0.68333333333333302</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="6" t="s">
+      <c r="A12" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C12" t="s">
@@ -2664,10 +2661,10 @@
       <c r="E12" s="4">
         <v>0.78333333333333299</v>
       </c>
-      <c r="G12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="6" t="s">
+      <c r="G12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="7" t="s">
         <v>19</v>
       </c>
       <c r="I12" t="s">
@@ -2679,10 +2676,10 @@
       <c r="K12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="N12" s="6" t="s">
+      <c r="M12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N12" s="7" t="s">
         <v>19</v>
       </c>
       <c r="O12" t="s">
@@ -2696,8 +2693,8 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
       <c r="C13" t="s">
         <v>13</v>
       </c>
@@ -2707,8 +2704,8 @@
       <c r="E13" s="4">
         <v>0.76666666666666605</v>
       </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
       <c r="I13" t="s">
         <v>13</v>
       </c>
@@ -2718,8 +2715,8 @@
       <c r="K13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
       <c r="O13" t="s">
         <v>13</v>
       </c>
@@ -2731,8 +2728,8 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
       <c r="C14" t="s">
         <v>14</v>
       </c>
@@ -2742,8 +2739,8 @@
       <c r="E14" s="4">
         <v>0.76666666666666605</v>
       </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
       <c r="I14" t="s">
         <v>14</v>
       </c>
@@ -2753,8 +2750,8 @@
       <c r="K14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
       <c r="O14" t="s">
         <v>14</v>
       </c>
@@ -2766,10 +2763,10 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="6" t="s">
+      <c r="A15" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C15" t="s">
@@ -2781,10 +2778,10 @@
       <c r="E15" s="4">
         <v>0.65</v>
       </c>
-      <c r="G15" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="H15" s="6" t="s">
+      <c r="G15" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="7" t="s">
         <v>21</v>
       </c>
       <c r="I15" t="s">
@@ -2796,25 +2793,25 @@
       <c r="K15" s="5">
         <v>0.73333333333333295</v>
       </c>
-      <c r="M15" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="N15" s="6" t="s">
+      <c r="M15" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="N15" s="7" t="s">
         <v>21</v>
       </c>
       <c r="O15" t="s">
         <v>10</v>
       </c>
       <c r="P15" s="5">
-        <v>1</v>
+        <v>0.99285714285714199</v>
       </c>
       <c r="Q15" s="5">
-        <v>0.66666666666666596</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
       <c r="C16" t="s">
         <v>13</v>
       </c>
@@ -2824,8 +2821,8 @@
       <c r="E16" s="4">
         <v>0.6</v>
       </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
       <c r="I16" t="s">
         <v>13</v>
       </c>
@@ -2835,8 +2832,8 @@
       <c r="K16" s="5">
         <v>0.7</v>
       </c>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
       <c r="O16" t="s">
         <v>13</v>
       </c>
@@ -2848,8 +2845,8 @@
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
       <c r="C17" t="s">
         <v>14</v>
       </c>
@@ -2859,8 +2856,8 @@
       <c r="E17" s="4">
         <v>0.63333333333333297</v>
       </c>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
       <c r="I17" t="s">
         <v>14</v>
       </c>
@@ -2868,8 +2865,8 @@
         <v>12</v>
       </c>
       <c r="K17" s="5"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
       <c r="O17" t="s">
         <v>14</v>
       </c>
@@ -2877,14 +2874,14 @@
         <v>1</v>
       </c>
       <c r="Q17" s="5">
-        <v>0.66666666666666596</v>
+        <v>0.68333333333333302</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="6" t="s">
+      <c r="A18" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>23</v>
       </c>
       <c r="C18" t="s">
@@ -2896,10 +2893,10 @@
       <c r="E18" s="4">
         <v>0.75</v>
       </c>
-      <c r="G18" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H18" s="6" t="s">
+      <c r="G18" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="7" t="s">
         <v>23</v>
       </c>
       <c r="I18" t="s">
@@ -2911,10 +2908,10 @@
       <c r="K18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M18" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="N18" s="6" t="s">
+      <c r="M18" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N18" s="7" t="s">
         <v>23</v>
       </c>
       <c r="O18" t="s">
@@ -2928,8 +2925,8 @@
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
       <c r="C19" t="s">
         <v>13</v>
       </c>
@@ -2939,8 +2936,8 @@
       <c r="E19" s="4">
         <v>0.75</v>
       </c>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
       <c r="I19" t="s">
         <v>13</v>
       </c>
@@ -2950,8 +2947,8 @@
       <c r="K19" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
       <c r="O19" t="s">
         <v>13</v>
       </c>
@@ -2963,8 +2960,8 @@
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
       <c r="C20" t="s">
         <v>14</v>
       </c>
@@ -2974,8 +2971,8 @@
       <c r="E20" s="4">
         <v>0.76666666666666605</v>
       </c>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
       <c r="I20" t="s">
         <v>14</v>
       </c>
@@ -2985,8 +2982,8 @@
       <c r="K20" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
       <c r="O20" t="s">
         <v>14</v>
       </c>
@@ -2999,15 +2996,26 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="M1:Q1"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="G3:G5"/>
-    <mergeCell ref="G6:G8"/>
-    <mergeCell ref="M3:M5"/>
-    <mergeCell ref="M6:M8"/>
+    <mergeCell ref="M9:M11"/>
+    <mergeCell ref="M12:M14"/>
+    <mergeCell ref="M15:M17"/>
+    <mergeCell ref="M18:M20"/>
+    <mergeCell ref="N3:N5"/>
+    <mergeCell ref="N6:N8"/>
+    <mergeCell ref="N9:N11"/>
+    <mergeCell ref="N12:N14"/>
+    <mergeCell ref="N15:N17"/>
+    <mergeCell ref="N18:N20"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="G12:G14"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="H3:H5"/>
+    <mergeCell ref="H6:H8"/>
+    <mergeCell ref="H9:H11"/>
+    <mergeCell ref="H12:H14"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="H18:H20"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A15:A17"/>
@@ -3018,26 +3026,15 @@
     <mergeCell ref="B12:B14"/>
     <mergeCell ref="B15:B17"/>
     <mergeCell ref="B18:B20"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="G12:G14"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="H3:H5"/>
-    <mergeCell ref="H6:H8"/>
-    <mergeCell ref="H9:H11"/>
-    <mergeCell ref="H12:H14"/>
-    <mergeCell ref="H15:H17"/>
-    <mergeCell ref="H18:H20"/>
-    <mergeCell ref="M9:M11"/>
-    <mergeCell ref="M12:M14"/>
-    <mergeCell ref="M15:M17"/>
-    <mergeCell ref="M18:M20"/>
-    <mergeCell ref="N3:N5"/>
-    <mergeCell ref="N6:N8"/>
-    <mergeCell ref="N9:N11"/>
-    <mergeCell ref="N12:N14"/>
-    <mergeCell ref="N15:N17"/>
-    <mergeCell ref="N18:N20"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="M1:Q1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="G6:G8"/>
+    <mergeCell ref="M3:M5"/>
+    <mergeCell ref="M6:M8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3047,7 +3044,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -3071,27 +3068,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="G1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="M1" s="7" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="G1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="M1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -3141,7 +3138,7 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
+      <c r="A3" s="7"/>
       <c r="B3" s="8" t="s">
         <v>9</v>
       </c>
@@ -3152,7 +3149,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="3"/>
-      <c r="G3" s="6"/>
+      <c r="G3" s="7"/>
       <c r="H3" s="8" t="s">
         <v>9</v>
       </c>
@@ -3163,7 +3160,7 @@
         <v>12</v>
       </c>
       <c r="K3" s="3"/>
-      <c r="M3" s="6"/>
+      <c r="M3" s="7"/>
       <c r="N3" s="8" t="s">
         <v>9</v>
       </c>
@@ -3176,7 +3173,7 @@
       <c r="Q3" s="3"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="8"/>
       <c r="C4" t="s">
         <v>13</v>
@@ -3185,7 +3182,7 @@
         <v>12</v>
       </c>
       <c r="E4" s="3"/>
-      <c r="G4" s="6"/>
+      <c r="G4" s="7"/>
       <c r="H4" s="8"/>
       <c r="I4" t="s">
         <v>13</v>
@@ -3194,7 +3191,7 @@
         <v>12</v>
       </c>
       <c r="K4" s="3"/>
-      <c r="M4" s="6"/>
+      <c r="M4" s="7"/>
       <c r="N4" s="8"/>
       <c r="O4" t="s">
         <v>13</v>
@@ -3205,7 +3202,7 @@
       <c r="Q4" s="3"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="8"/>
       <c r="C5" t="s">
         <v>14</v>
@@ -3214,7 +3211,7 @@
         <v>12</v>
       </c>
       <c r="E5" s="3"/>
-      <c r="G5" s="6"/>
+      <c r="G5" s="7"/>
       <c r="H5" s="8"/>
       <c r="I5" t="s">
         <v>14</v>
@@ -3223,7 +3220,7 @@
         <v>12</v>
       </c>
       <c r="K5" s="3"/>
-      <c r="M5" s="6"/>
+      <c r="M5" s="7"/>
       <c r="N5" s="8"/>
       <c r="O5" t="s">
         <v>14</v>
@@ -3234,8 +3231,8 @@
       <c r="Q5" s="3"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C6" t="s">
@@ -3245,8 +3242,8 @@
         <v>12</v>
       </c>
       <c r="E6" s="3"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6" t="s">
+      <c r="G6" s="7"/>
+      <c r="H6" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I6" t="s">
@@ -3256,8 +3253,8 @@
         <v>12</v>
       </c>
       <c r="K6" s="3"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6" t="s">
+      <c r="M6" s="7"/>
+      <c r="N6" s="7" t="s">
         <v>15</v>
       </c>
       <c r="O6" t="s">
@@ -3269,8 +3266,8 @@
       <c r="Q6" s="3"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
       <c r="C7" t="s">
         <v>13</v>
       </c>
@@ -3278,8 +3275,8 @@
         <v>12</v>
       </c>
       <c r="E7" s="3"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
       <c r="I7" t="s">
         <v>13</v>
       </c>
@@ -3287,8 +3284,8 @@
         <v>12</v>
       </c>
       <c r="K7" s="3"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
       <c r="O7" t="s">
         <v>13</v>
       </c>
@@ -3298,8 +3295,8 @@
       <c r="Q7" s="3"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
       <c r="C8" t="s">
         <v>14</v>
       </c>
@@ -3307,8 +3304,8 @@
         <v>12</v>
       </c>
       <c r="E8" s="3"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
       <c r="I8" t="s">
         <v>14</v>
       </c>
@@ -3316,8 +3313,8 @@
         <v>12</v>
       </c>
       <c r="K8" s="3"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
       <c r="O8" t="s">
         <v>14</v>
       </c>
@@ -3327,8 +3324,8 @@
       <c r="Q8" s="3"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6" t="s">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C9" t="s">
@@ -3338,8 +3335,8 @@
         <v>12</v>
       </c>
       <c r="E9" s="3"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6" t="s">
+      <c r="G9" s="7"/>
+      <c r="H9" s="7" t="s">
         <v>17</v>
       </c>
       <c r="I9" t="s">
@@ -3349,8 +3346,8 @@
         <v>12</v>
       </c>
       <c r="K9" s="3"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6" t="s">
+      <c r="M9" s="7"/>
+      <c r="N9" s="7" t="s">
         <v>17</v>
       </c>
       <c r="O9" t="s">
@@ -3362,8 +3359,8 @@
       <c r="Q9" s="3"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
       <c r="C10" t="s">
         <v>13</v>
       </c>
@@ -3371,8 +3368,8 @@
         <v>12</v>
       </c>
       <c r="E10" s="3"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
       <c r="I10" t="s">
         <v>13</v>
       </c>
@@ -3380,8 +3377,8 @@
         <v>12</v>
       </c>
       <c r="K10" s="3"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
       <c r="O10" t="s">
         <v>13</v>
       </c>
@@ -3391,8 +3388,8 @@
       <c r="Q10" s="3"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
       <c r="C11" t="s">
         <v>14</v>
       </c>
@@ -3400,8 +3397,8 @@
         <v>12</v>
       </c>
       <c r="E11" s="3"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
       <c r="I11" t="s">
         <v>14</v>
       </c>
@@ -3409,8 +3406,8 @@
         <v>12</v>
       </c>
       <c r="K11" s="3"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
       <c r="O11" t="s">
         <v>14</v>
       </c>
@@ -3420,8 +3417,8 @@
       <c r="Q11" s="3"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6" t="s">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C12" t="s">
@@ -3431,8 +3428,8 @@
         <v>12</v>
       </c>
       <c r="E12" s="3"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6" t="s">
+      <c r="G12" s="7"/>
+      <c r="H12" s="7" t="s">
         <v>19</v>
       </c>
       <c r="I12" t="s">
@@ -3442,8 +3439,8 @@
         <v>12</v>
       </c>
       <c r="K12" s="3"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6" t="s">
+      <c r="M12" s="7"/>
+      <c r="N12" s="7" t="s">
         <v>19</v>
       </c>
       <c r="O12" t="s">
@@ -3455,8 +3452,8 @@
       <c r="Q12" s="3"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
       <c r="C13" t="s">
         <v>13</v>
       </c>
@@ -3464,8 +3461,8 @@
         <v>12</v>
       </c>
       <c r="E13" s="3"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
       <c r="I13" t="s">
         <v>13</v>
       </c>
@@ -3473,8 +3470,8 @@
         <v>12</v>
       </c>
       <c r="K13" s="3"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
       <c r="O13" t="s">
         <v>13</v>
       </c>
@@ -3484,8 +3481,8 @@
       <c r="Q13" s="3"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
       <c r="C14" t="s">
         <v>14</v>
       </c>
@@ -3493,8 +3490,8 @@
         <v>12</v>
       </c>
       <c r="E14" s="3"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
       <c r="I14" t="s">
         <v>14</v>
       </c>
@@ -3502,8 +3499,8 @@
         <v>12</v>
       </c>
       <c r="K14" s="3"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
       <c r="O14" t="s">
         <v>14</v>
       </c>
@@ -3513,8 +3510,8 @@
       <c r="Q14" s="3"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6" t="s">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C15" t="s">
@@ -3524,8 +3521,8 @@
         <v>12</v>
       </c>
       <c r="E15" s="3"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6" t="s">
+      <c r="G15" s="7"/>
+      <c r="H15" s="7" t="s">
         <v>21</v>
       </c>
       <c r="I15" t="s">
@@ -3535,8 +3532,8 @@
         <v>12</v>
       </c>
       <c r="K15" s="3"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6" t="s">
+      <c r="M15" s="7"/>
+      <c r="N15" s="7" t="s">
         <v>21</v>
       </c>
       <c r="O15" t="s">
@@ -3548,8 +3545,8 @@
       <c r="Q15" s="3"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
       <c r="C16" t="s">
         <v>13</v>
       </c>
@@ -3557,8 +3554,8 @@
         <v>12</v>
       </c>
       <c r="E16" s="3"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
       <c r="I16" t="s">
         <v>13</v>
       </c>
@@ -3566,8 +3563,8 @@
         <v>12</v>
       </c>
       <c r="K16" s="3"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
       <c r="O16" t="s">
         <v>13</v>
       </c>
@@ -3577,8 +3574,8 @@
       <c r="Q16" s="3"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
       <c r="C17" t="s">
         <v>14</v>
       </c>
@@ -3586,8 +3583,8 @@
         <v>12</v>
       </c>
       <c r="E17" s="3"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
       <c r="I17" t="s">
         <v>14</v>
       </c>
@@ -3595,8 +3592,8 @@
         <v>12</v>
       </c>
       <c r="K17" s="3"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
       <c r="O17" t="s">
         <v>14</v>
       </c>
@@ -3606,8 +3603,8 @@
       <c r="Q17" s="3"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6" t="s">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7" t="s">
         <v>23</v>
       </c>
       <c r="C18" t="s">
@@ -3617,8 +3614,8 @@
         <v>12</v>
       </c>
       <c r="E18" s="3"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6" t="s">
+      <c r="G18" s="7"/>
+      <c r="H18" s="7" t="s">
         <v>23</v>
       </c>
       <c r="I18" t="s">
@@ -3628,8 +3625,8 @@
         <v>12</v>
       </c>
       <c r="K18" s="3"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6" t="s">
+      <c r="M18" s="7"/>
+      <c r="N18" s="7" t="s">
         <v>23</v>
       </c>
       <c r="O18" t="s">
@@ -3641,8 +3638,8 @@
       <c r="Q18" s="3"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
       <c r="C19" t="s">
         <v>13</v>
       </c>
@@ -3650,8 +3647,8 @@
         <v>12</v>
       </c>
       <c r="E19" s="3"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
       <c r="I19" t="s">
         <v>13</v>
       </c>
@@ -3659,8 +3656,8 @@
         <v>12</v>
       </c>
       <c r="K19" s="3"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
       <c r="O19" t="s">
         <v>13</v>
       </c>
@@ -3670,8 +3667,8 @@
       <c r="Q19" s="3"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
       <c r="C20" t="s">
         <v>14</v>
       </c>
@@ -3679,8 +3676,8 @@
         <v>12</v>
       </c>
       <c r="E20" s="3"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
       <c r="I20" t="s">
         <v>14</v>
       </c>
@@ -3688,8 +3685,8 @@
         <v>12</v>
       </c>
       <c r="K20" s="3"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
       <c r="O20" t="s">
         <v>14</v>
       </c>
@@ -3700,15 +3697,26 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="M1:Q1"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="G3:G5"/>
-    <mergeCell ref="G6:G8"/>
-    <mergeCell ref="M3:M5"/>
-    <mergeCell ref="M6:M8"/>
+    <mergeCell ref="M9:M11"/>
+    <mergeCell ref="M12:M14"/>
+    <mergeCell ref="M15:M17"/>
+    <mergeCell ref="M18:M20"/>
+    <mergeCell ref="N3:N5"/>
+    <mergeCell ref="N6:N8"/>
+    <mergeCell ref="N9:N11"/>
+    <mergeCell ref="N12:N14"/>
+    <mergeCell ref="N15:N17"/>
+    <mergeCell ref="N18:N20"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="G12:G14"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="H3:H5"/>
+    <mergeCell ref="H6:H8"/>
+    <mergeCell ref="H9:H11"/>
+    <mergeCell ref="H12:H14"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="H18:H20"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A15:A17"/>
@@ -3719,26 +3727,15 @@
     <mergeCell ref="B12:B14"/>
     <mergeCell ref="B15:B17"/>
     <mergeCell ref="B18:B20"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="G12:G14"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="H3:H5"/>
-    <mergeCell ref="H6:H8"/>
-    <mergeCell ref="H9:H11"/>
-    <mergeCell ref="H12:H14"/>
-    <mergeCell ref="H15:H17"/>
-    <mergeCell ref="H18:H20"/>
-    <mergeCell ref="M9:M11"/>
-    <mergeCell ref="M12:M14"/>
-    <mergeCell ref="M15:M17"/>
-    <mergeCell ref="M18:M20"/>
-    <mergeCell ref="N3:N5"/>
-    <mergeCell ref="N6:N8"/>
-    <mergeCell ref="N9:N11"/>
-    <mergeCell ref="N12:N14"/>
-    <mergeCell ref="N15:N17"/>
-    <mergeCell ref="N18:N20"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="M1:Q1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="G6:G8"/>
+    <mergeCell ref="M3:M5"/>
+    <mergeCell ref="M6:M8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>